<commit_message>
add Copeland air regressions
</commit_message>
<xml_diff>
--- a/N. Umpqua 2024 Temperature Summary.xlsx
+++ b/N. Umpqua 2024 Temperature Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\NUmpqua_TempAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983F88E-B2AA-4225-AAA6-E86C4E67C6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E232EE-5AED-4F3B-A5D7-733BB54F3489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MDMTDaysAbove20" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="57">
   <si>
     <t>Logger ID</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>F-statistic: 0.5375 on 1 and 11 DF,  p-value: 0.4788</t>
+  </si>
+  <si>
+    <t>MEAN TEMP AIR WATER REGRESSIONS (Air Temp Baseline @ Copeland Cr.)</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -428,6 +429,8 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1167,15 +1170,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
@@ -1184,18 +1187,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="12.75">
       <c r="A3" s="1" t="s">
@@ -1646,18 +1649,18 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="12.75">
       <c r="A20" s="1" t="s">
@@ -2106,6 +2109,20 @@
       <c r="J33" s="12">
         <v>0.83177789999999996</v>
       </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A36" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10" ht="12.75">
       <c r="A37" s="10"/>
@@ -2118,10 +2135,103 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
     </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="4">
+        <v>43.266770000000001</v>
+      </c>
+      <c r="D39" s="4">
+        <v>-122.5198</v>
+      </c>
+      <c r="E39" s="12">
+        <v>7.2084200000000003</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.30706</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.76570000000000005</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0.52059999999999995</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="12">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A40" s="4">
+        <v>21679163</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="4">
+        <v>43.28472</v>
+      </c>
+      <c r="D40" s="4">
+        <v>-122.4706</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A41" s="4">
+        <v>21679182</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="4">
+        <v>43.266800000000003</v>
+      </c>
+      <c r="D41" s="4">
+        <v>-122.51949999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A36:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2131,179 +2241,179 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D679502E-A66B-432A-BBA5-7331ECBEF912}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="20"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="20"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="17"/>
+      <c r="A5" s="15"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="17"/>
+      <c r="A9" s="15"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="17"/>
+      <c r="A16" s="15"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="17"/>
+      <c r="A26" s="15"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="17"/>
+      <c r="A30" s="15"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="16" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="17"/>
+      <c r="A37" s="15"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="17" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>